<commit_message>
Pasta com as tabelas geradas
</commit_message>
<xml_diff>
--- a/Listas de Compras/TabelaOfertas.xlsx
+++ b/Listas de Compras/TabelaOfertas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>Produto</t>
   </si>
@@ -25,217 +25,253 @@
     <t>Link</t>
   </si>
   <si>
-    <t>iphone 12 64gb - branco - estou zerado</t>
+    <t>vitrine: iphone 12 apple 64gb roxo tela 61 câmera traseira 12mp ios</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb - azul - estou zerado</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb - roxo - estou zerado</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb - preto - estou zerado</t>
+  </si>
+  <si>
+    <t>usado: iphone 12 64gb preto bom - trocafone</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb roxo - swap</t>
+  </si>
+  <si>
+    <t>(seminovo) iphone 12 apple preto 64gb</t>
+  </si>
+  <si>
+    <t>apple iphone 12 64gb vitrine com brinde</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb preto - swap</t>
+  </si>
+  <si>
+    <t>(seminovo) iphone 12 apple azul 64gb</t>
+  </si>
+  <si>
+    <t>(seminovo) iphone 12 apple verde 64gb</t>
   </si>
   <si>
     <t>iphone xr 64gb branco com tela de 61 4g e câmera de 12 mp - mh6n3br/a</t>
   </si>
   <si>
-    <t>vitrine: iphone 12 apple 64gb preto tela 61 câmera traseira dupla 12mp ios</t>
-  </si>
-  <si>
-    <t>iphone 12 64gb - preto - estou zerado</t>
-  </si>
-  <si>
-    <t>iphone 12 64gb - roxo - estou zerado</t>
-  </si>
-  <si>
-    <t>vitrine: iphone 12 apple 64gb roxo tela 61 câmera traseira 12mp ios</t>
-  </si>
-  <si>
-    <t>usado: iphone 12 64gb preto bom - trocafone</t>
-  </si>
-  <si>
-    <t>(seminovo) iphone 12 apple preto 64gb</t>
-  </si>
-  <si>
-    <t>(seminovo) iphone 12 apple verde 64gb</t>
-  </si>
-  <si>
-    <t>iphone 12 64gb preto - swap</t>
-  </si>
-  <si>
-    <t>(seminovo) iphone 12 apple azul 64gb</t>
+    <t>(seminovo) iphone 12 apple branco 64gb</t>
+  </si>
+  <si>
+    <t>apple iphone 12 64gb azul vitrine 10x /juros</t>
+  </si>
+  <si>
+    <t>(seminovo) iphone 12 apple (product)red  64gb</t>
+  </si>
+  <si>
+    <t>iphone 12 64gb azul - swap</t>
+  </si>
+  <si>
+    <t>iphone xr 64gb/128gb semi-novos 90% a 100% bateria</t>
   </si>
   <si>
     <t>iphone 12 64gb branco - swap</t>
   </si>
   <si>
-    <t>iphone 12 64gb azul - swap</t>
-  </si>
-  <si>
-    <t>(seminovo) iphone 12 apple branco 64gb</t>
-  </si>
-  <si>
-    <t>iphone 12 64gb roxo - swap</t>
-  </si>
-  <si>
-    <t>(seminovo) iphone 12 apple (product)red  64gb</t>
-  </si>
-  <si>
     <t>smartphone apple iphone 12 64gb câmera dupla</t>
   </si>
   <si>
+    <t>placa de vídeo gainward geforce rtx 3060 ti 8gb ghost gddr6 - ne6306t019p2-190ab</t>
+  </si>
+  <si>
     <t>placa de video msi geforce rtx 3060 gaming x 12gb gddr6 192</t>
   </si>
   <si>
-    <t>placa de vídeo geforce rtx 3060 v2 dual 12gb gddr6 asus</t>
-  </si>
-  <si>
-    <t>placa de vídeo gainward geforce rtx 3060 ti 8gb ghost gddr6 - ne6306t019p2-190ab</t>
+    <t>placa de vídeo gigabyte gaming oc 12gb geforce rtx3060 gddr6 / rgb - gv ...</t>
   </si>
   <si>
     <t>placa de vídeo rtx 3060ti 8gb zerada palit</t>
   </si>
   <si>
+    <t>pc gamer enifler intel core i7 rtx 3060 16gb ram ssd 480gb black hawk</t>
+  </si>
+  <si>
     <t>placa de vídeo evga geforce rtx 3060 xc gaming 12 gb gddr6</t>
   </si>
   <si>
-    <t>placa de vídeo gigabyte gaming oc 12gb geforce rtx3060 gddr6 / rgb - gv ...</t>
-  </si>
-  <si>
-    <t>gigabyte geforce rtx 3060 ti gaming oc 8g (rev2.0) card de windforce 3x lhr 8gb ...</t>
+    <t>pc gamer t-gamer hawk intel i5 10400f / nvidia geforce rtx 3060 / 8gb ddr4 / ssd ...</t>
+  </si>
+  <si>
+    <t>pc gamer t-gamer flux amd ryzen 5 5500 / nvidia geforce rtx 3060 / 8gb ddr4 / ssd ...</t>
   </si>
   <si>
     <t>gigabyte baru ga aorus geforce rtx 3060 ti gaming vision eagle 12g gddr6 256 bits ...</t>
   </si>
   <si>
+    <t>pc gamer t-gamer vector ryzen 5 4600g / nvidia geforce rtx 3060 / 8gb ddr4 / ssd ...</t>
+  </si>
+  <si>
     <t>force rtx 3060 gaming z trio placas gráficas raphic card 12g lhr 12 gb gddr6 192 ...</t>
   </si>
   <si>
     <t>placa de video nvidia geforce rtx 3060 12 gb gddr6 192 bits asus tuf-rtx3060-o12g-gaming</t>
   </si>
   <si>
-    <t>3059.10</t>
-  </si>
-  <si>
-    <t>3059.15</t>
-  </si>
-  <si>
-    <t>3295.55</t>
-  </si>
-  <si>
-    <t>3209.00</t>
-  </si>
-  <si>
-    <t>3144.15</t>
-  </si>
-  <si>
-    <t>3219.00</t>
-  </si>
-  <si>
-    <t>3098.00</t>
-  </si>
-  <si>
-    <t>3259.00</t>
-  </si>
-  <si>
-    <t>4259.00</t>
-  </si>
-  <si>
-    <t>4336.65</t>
-  </si>
-  <si>
-    <t>4257.70</t>
-  </si>
-  <si>
-    <t>4000.00</t>
-  </si>
-  <si>
-    <t>4123.00</t>
-  </si>
-  <si>
-    <t>4050.00</t>
-  </si>
-  <si>
-    <t>4249.00</t>
-  </si>
-  <si>
-    <t>4019.28</t>
-  </si>
-  <si>
-    <t>4106.64</t>
-  </si>
-  <si>
-    <t>4441.10</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/4953060183210391573?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA1YJWDJAWgBcAB4AIABlAGIAcoEkgEDMC40mAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:15949918359662290038_0,pid:13016743435382930939,rsk:PC_11630641001267601036&amp;sa=X&amp;ved=0ahUKEwjy2cv9qMP-AhXfKrkGHX_-CYAQ8gII1g4oAA</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/7578846592293227918?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA1YJWDJAWgBcAB4AIABlAGIAcoEkgEDMC40mAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:419100260293419769_0,pid:12290781261691180637,rsk:PC_15653290272112071452&amp;sa=X&amp;ved=0ahUKEwjy2cv9qMP-AhXfKrkGHX_-CYAQ8gII2Q8oAA</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/10731725505291757596?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA1YJWDJAWgBcAB4AIABlAGIAcoEkgEDMC40mAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:2441934400410085411_0,pid:16674502977534662409,rsk:PC_14074616196041694734&amp;sa=X&amp;ved=0ahUKEwjy2cv9qMP-AhXfKrkGHX_-CYAQ8gIImRAoAA</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/925660058154905741?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA1YJWDJAWgBcAB4AIABlAGIAcoEkgEDMC40mAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:3327467532283076065_0,pid:17698061794397978400&amp;sa=X&amp;ved=0ahUKEwjy2cv9qMP-AhXfKrkGHX_-CYAQ8gIIkxIoAA</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/1409198851555036304?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA1YJWDJAWgBcAB4AIABlAGIAcoEkgEDMC40mAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:14066938966366365827_0,pid:5070126177312031027&amp;sa=X&amp;ved=0ahUKEwjy2cv9qMP-AhXfKrkGHX_-CYAQ8gIIyhQoAA</t>
-  </si>
-  <si>
-    <t>https://www.carrefour.com.br/vitrine-iphone-12-apple-64gb-roxo-tela-61-camera-traseira-12mp-ios-mp932337971/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwj31ev_qMP-AhXTCrkGHVsPAbU4PBDVKQi5DSgA&amp;usg=AOvVaw3LFaWXFLI8PlnbW7RZru7u</t>
-  </si>
-  <si>
-    <t>https://www.carrefour.com.br/usado-iphone-12-64gb-preto-bom-trocafone-mp930839701/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwj31ev_qMP-AhXTCrkGHVsPAbU4PBDVKQjyECgA&amp;usg=AOvVaw0EUEQU-K7qYdwcSnkRmBxd</t>
-  </si>
-  <si>
-    <t>https://www.taqi.com.br/seminovo-iphone12-64gbpreto-internacional/220672%3Fsrsltid%3DAfAwrE6A9lTGVs-UufudqLRvbDcIgM88v3rtuHBmCfZLAYMBpuRNqR4H3-Y&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwj31ev_qMP-AhXTCrkGHVsPAbU4PBDVKQiIEygA&amp;usg=AOvVaw12jqBA-p9BASEFr8Wl6Qaf</t>
-  </si>
-  <si>
-    <t>https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-verde-taqi/222821%3Fsrsltid%3DAfAwrE7m-9QtgYv7qnWgsYStQg4BKHTeuEM_O3CoJ8d5MhWDfzDVaevR6Nw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwj31ev_qMP-AhXTCrkGHVsPAbU4PBDVKQjWEygA&amp;usg=AOvVaw1egQN9Z66AczPHIehkJCAz</t>
-  </si>
-  <si>
-    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-preto-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE4vXUskfiSQepz-3n9Lm5vdpVDWhyf70IJIGIJuXCTlueeHbt4y3aI&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwj31ev_qMP-AhXTCrkGHVsPAbU4PBDVKQjRFCgA&amp;usg=AOvVaw3aCNzGlvrU6zOsmG45gx_2</t>
-  </si>
-  <si>
-    <t>https://www.taqi.com.br/seminovo-iphone12-apple-azul64gb-nacional/220673%3Fsrsltid%3DAfAwrE7Cqsu4Gh76H9DfmDX0doRTRwN8RUgzh4Q65LBk8KDl3D7bZYGyoHM&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwi2rcGCqcP-AhU_IrkGHYcKB5E4eBDVKQj9DCgA&amp;usg=AOvVaw3q4lva4I38BBHXnO1X-2FF</t>
-  </si>
-  <si>
-    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-branco-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE51--0_7zuC6H1udpqnDW5bP2Yp1kKlkS8EjpodRbZzDKq76U7eWPY&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwi2rcGCqcP-AhU_IrkGHYcKB5E4eBDVKQibDSgA&amp;usg=AOvVaw2tUXJp9hUOp9M51Ss_g2S9</t>
-  </si>
-  <si>
-    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-azul-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE7KqdbUq_Py3LpgzzZ9_ix5PT_yMLFgopz9djLDc2_ga8yw28pSgrs&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwi2rcGCqcP-AhU_IrkGHYcKB5E4eBDVKQiJDigA&amp;usg=AOvVaw2_nAHaTGPCT6JRiuZDmsRZ</t>
-  </si>
-  <si>
-    <t>https://www.taqi.com.br/seminovo-apple-iphone12-64gb-internacional-taqi/222815%3Fsrsltid%3DAfAwrE7tOdeM3QI2hYkl8MEIw31Jk3nn9CJJZB0oHYqmSXKKRYSI5qYDFRg&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwi2rcGCqcP-AhU_IrkGHYcKB5E4eBDVKQinDigA&amp;usg=AOvVaw2LSh1ki12vzFcZ0o_00szv</t>
-  </si>
-  <si>
-    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-roxo-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE5X6qwoumQUX3LE00EBjK_n-xUQh_ar5cuW47KqGRAYygaxGr1MJyY&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwi2rcGCqcP-AhU_IrkGHYcKB5E4eBDVKQj2DigA&amp;usg=AOvVaw3SmoaUc_lxM6c3_YsHclRd</t>
-  </si>
-  <si>
-    <t>https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-productred/221656%3Fsrsltid%3DAfAwrE6-OVlbPxtuPZhWzcvVG6mKyUZ5GJpFIkFfNP5nQ2PpNGt1Lx5nskA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwi2rcGCqcP-AhU_IrkGHYcKB5E4eBDVKQjaESgA&amp;usg=AOvVaw2QXGFEaizCVuy5BO-k6Jvq</t>
+    <t>3.295,55</t>
+  </si>
+  <si>
+    <t>3.059,10</t>
+  </si>
+  <si>
+    <t>3.209,00</t>
+  </si>
+  <si>
+    <t>3.098,00</t>
+  </si>
+  <si>
+    <t>3.144,15</t>
+  </si>
+  <si>
+    <t>3.499,20</t>
+  </si>
+  <si>
+    <t>3.219,00</t>
+  </si>
+  <si>
+    <t>3.059,15</t>
+  </si>
+  <si>
+    <t>3.100,99</t>
+  </si>
+  <si>
+    <t>3.173,00</t>
+  </si>
+  <si>
+    <t>4.257,70</t>
+  </si>
+  <si>
+    <t>4.259,00</t>
+  </si>
+  <si>
+    <t>4.050,00</t>
+  </si>
+  <si>
+    <t>4.000,00</t>
+  </si>
+  <si>
+    <t>4.171,82</t>
+  </si>
+  <si>
+    <t>4.123,00</t>
+  </si>
+  <si>
+    <t>4.450,80</t>
+  </si>
+  <si>
+    <t>4.355,79</t>
+  </si>
+  <si>
+    <t>4.019,28</t>
+  </si>
+  <si>
+    <t>4.414,89</t>
+  </si>
+  <si>
+    <t>4.106,64</t>
+  </si>
+  <si>
+    <t>4.441,10</t>
+  </si>
+  <si>
+    <t>https://www.carrefour.com.br/vitrine-iphone-12-apple-64gb-roxo-tela-61-camera-traseira-12mp-ios-mp932337971/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkInQwoAA&amp;usg=AOvVaw1HH_a07EZx6LXR9n7fiKXa</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/357344828079836893?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUAxYJmBFaABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:10360267435465518254_0,pid:4387230182954649532,rsk:PC_11630641001267601036&amp;sa=X&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q8gIIrQwoAA</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/1409198851555036304?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUAxYJmBFaABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:14066938966366365827_0,pid:5070126177312031027&amp;sa=X&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q8gIIzwwoAA</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/925660058154905741?hl=pt-BR&amp;psb=1&amp;q=iphone+12+64gb&amp;oq=iphone+12+64gb&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUAxYJmBFaABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:3327467532283076065_0,pid:17698061794397978400&amp;sa=X&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q8gIIgA0oAA</t>
+  </si>
+  <si>
+    <t>https://www.carrefour.com.br/usado-iphone-12-64gb-preto-bom-trocafone-mp930839701/p&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkIkA0oAA&amp;usg=AOvVaw2v0LX5Z6VHNHbLoSMhKQoh</t>
+  </si>
+  <si>
+    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-roxo-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE55-tKSlEBR46XyFms743inPMCsRwiLY8HzWVIdwJorSVKM4WseqPw&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkIsA4oAA&amp;usg=AOvVaw0KOGD9TxKly0g5QWQzG042</t>
+  </si>
+  <si>
+    <t>https://www.taqi.com.br/seminovo-usado-apple-iphone-12-preto-nacional/221635%3Fsrsltid%3DAfAwrE7NnpoSV5soJZuCs0FD2V0PkR3hd8XeNVXOhHOhK8dqSdLZ89kUktU&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkI7w4oAA&amp;usg=AOvVaw3IBzw8v-XHnjz3G2zJiC2M</t>
+  </si>
+  <si>
+    <t>https://produto.mercadolivre.com.br/MLB-3265035765-apple-iphone-12-64gb-vitrine-promoco-com-brinde-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkIyg8oAA&amp;usg=AOvVaw3Ztp5VjBNS-XdptY0LIY02</t>
+  </si>
+  <si>
+    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-preto-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE6QHOzuRqr3qbUqSQ-8DDgk8UWcuEseYAH9FAPXrIoPMXzzlD4vAKo&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkIlREoAA&amp;usg=AOvVaw0GgfG8ohs6n8Ofrtc69kDP</t>
+  </si>
+  <si>
+    <t>https://www.taqi.com.br/seminovo-iphone12-apple-azul64gb-nacional/220673%3Fsrsltid%3DAfAwrE4aVloUDC2pBVu9sDWDdQkY3gJKRKXgOJIL-FKwp_IQ5nJLyBICPJA&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiz-sjqsMP-AhXTnpUCHWZMA08Q1SkI1xIoAA&amp;usg=AOvVaw3fyMlIpfZtGcLuzQYHcrrM</t>
+  </si>
+  <si>
+    <t>https://www.taqi.com.br/seminovo-apple-iphone-12-64gb-verde-taqi/222821%3Fsrsltid%3DAfAwrE5xDxB-ESpv9KeL9YkfJar9bvCePhJXmxByEp7014acSqJxUOGbBiQ&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiSyOnssMP-AhWZs5UCHaC0AYs4PBDVKQiUDigA&amp;usg=AOvVaw2LoNwEYKRoB_blQwXLLtcY</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/7578846592293227918?q=iphone+12+64gb&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;prds=eto:419100260293419769_0,pid:12290781261691180637,rsk:PC_15653290272112071452&amp;sa=X&amp;ved=0ahUKEwiSyOnssMP-AhWZs5UCHaC0AYs4PBDyAgi_ECgA</t>
+  </si>
+  <si>
+    <t>https://www.taqi.com.br/seminovo-apple-iphone12-64gb-internacional-taqi/222815%3Fsrsltid%3DAfAwrE4slj_6mYgKZHyr5PxlfL7omSY_Y39dsvKwHo1K1Ts-Z9CE9iA2N2A&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiSyOnssMP-AhWZs5UCHaC0AYs4PBDVKQiZEigA&amp;usg=AOvVaw1_H21PSuLlXvbbKvoKcMm5</t>
+  </si>
+  <si>
+    <t>https://produto.mercadolivre.com.br/MLB-3460983776-apple-iphone-12-64gb-azul-vitrine-10x-juros-_JM%3Fmatt_tool%3D18956390%26utm_source%3Dgoogle_shopping%26utm_medium%3Dorganic&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiyyI_vsMP-AhXQq5UCHfyIBos4eBDVKQiRDSgA&amp;usg=AOvVaw3ZgwldEMJ42_mEA0WN9wgs</t>
+  </si>
+  <si>
+    <t>https://www.taqi.com.br/seminovo-apple-iphone-12-vermelho-64gb/221655%3Fsrsltid%3DAfAwrE4mbmwymVZaF89dlu8wABvZTf44X_vK747U0KecAX4kqVwrh9opJoc&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiyyI_vsMP-AhXQq5UCHfyIBos4eBDVKQjODSgA&amp;usg=AOvVaw2EGtGEthMusTQEobBCWc3D</t>
+  </si>
+  <si>
+    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-azul-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE7wmFc3qm9pWme5eGVNHmfEpZE890xH2cRc2yXU5lJeZXNAAQH0_v0&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjBtazxsMP-AhWopZUCHSsWAc04tAEQ1SkI7w4oAA&amp;usg=AOvVaw19HyJyffvVni1qJf4dY2W0</t>
+  </si>
+  <si>
+    <t>https://mercadodenovidades.com.br/produto/iphone-xr-64gb-128gb-semi-novo-90-a-100-bateria/%3Fattribute_pa_cor%3Dcoral-64gb&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjBtazxsMP-AhWopZUCHSsWAc04tAEQ1SkIihIoAA&amp;usg=AOvVaw0ccNt-acsz1b8L8xzpxseB</t>
+  </si>
+  <si>
+    <t>https://www.malibushop.com.br/iphones-semi-novos/iphones-swap/iphone-12-64gb-branco-swap%3Fparceiro%3D1538%26srsltid%3DAfAwrE56qWJaSZ6jlEyBAO2jK_MZrb6Ir3RybANO1sEJAbg3ZFVhBbc7hHs&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwj1iNfzsMP-AhVTqpUCHSUNDOA48AEQ1SkI0A4oAA&amp;usg=AOvVaw2FiZzwtDSniqUJNvs9pQyj</t>
   </si>
   <si>
     <t>https://www.buscape.com.br/celular/smartphone-apple-iphone-12-64gb-ios?_lc=88&amp;searchterm=iphone%2012%2064gb</t>
   </si>
   <si>
-    <t>https://www.google.com.br/shopping/product/6156775075873092315?hl=pt-BR&amp;psb=1&amp;q=rtx+3060&amp;oq=rtx+3060&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA5YH2A_aABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:6583861436975444040_0,pid:5505575770092825149,rsk:PC_15471865893957977821&amp;sa=X&amp;ved=0ahUKEwiGreaHqcP-AhWNDbkGHVflBSwQ8gIIkQ4oAA</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/11344474960073929217?hl=pt-BR&amp;psb=1&amp;q=rtx+3060&amp;oq=rtx+3060&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA5YH2A_aABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:7674385353818543150_0,pid:15806797841025520384,rsk:PC_14041847408802663274&amp;sa=X&amp;ved=0ahUKEwiGreaHqcP-AhWNDbkGHVflBSwQ8gIIlA8oAA</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/1907077153485232263?hl=pt-BR&amp;psb=1&amp;q=rtx+3060&amp;oq=rtx+3060&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUA5YH2A_aABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:2894199181455547027_0,pid:6578317445486695424,rsk:PC_2714968812938645094&amp;sa=X&amp;ved=0ahUKEwiGreaHqcP-AhWNDbkGHVflBSwQ8gIInBAoAA</t>
-  </si>
-  <si>
-    <t>https://shopee.com.br/product/304224916/16586755093&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiGreaHqcP-AhWNDbkGHVflBSwQ1SkI7REoAA&amp;usg=AOvVaw24YtZ8ggR6fQl6MFw2OSKZ</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/14305462128264014099?q=rtx+3060&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;dpr=1&amp;prds=eto:11665494753858532241_0,pid:9462093140828316906,rsk:PC_10875814643528672174&amp;sa=X&amp;ved=0ahUKEwiQzvmJqcP-AhUJL7kGHeRGAWc4PBDyAgiFECgA</t>
-  </si>
-  <si>
-    <t>https://www.casasbahia.com.br/placa-de-video-gigabyte-gaming-oc-12gb-geforce-rtx3060-gddr6-rgb-gv-n3060gaming-oc-12gd-1535614552/p/1535614552%3Futm_medium%3DCpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1535614552%26idLojista%3D192053%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjqypGMqcP-AhVwA7kGHY_mDxU4eBDVKQjzDCgA&amp;usg=AOvVaw3IT_LiNMENwZ1C6Lz6tHVE</t>
-  </si>
-  <si>
-    <t>https://www.google.com.br/shopping/product/13290798811256723727?q=rtx+3060&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;dpr=1&amp;prds=eto:16542550369473719393_0,pid:2355399741657646707,rsk:PC_3012995993088900538&amp;sa=X&amp;ved=0ahUKEwjqypGMqcP-AhVwA7kGHY_mDxU4eBDyAgjmDygA</t>
-  </si>
-  <si>
-    <t>https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004999142258.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjM6fWSqcP-AhXpF7kGHb7rBGs4rAIQ1SkIuAooAA&amp;usg=AOvVaw3kQrlAzvZFFwZlD-9-cANQ</t>
-  </si>
-  <si>
-    <t>https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005003484105534.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjbu9OXqcP-AhX9G7kGHUKHCPU4pAMQ1SkIvAooAA&amp;usg=AOvVaw1A4fRP16PiWts0kzX62dVy</t>
+    <t>https://www.google.com.br/shopping/product/1907077153485232263?hl=pt-BR&amp;psb=1&amp;q=rtx+3060&amp;oq=rtx+3060&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUAxYHWA-aABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:2894199181455547027_0,pid:6578317445486695424,rsk:PC_2714968812938645094&amp;sa=X&amp;ved=0ahUKEwjK95j9sMP-AhV-r5UCHcT0DKwQ8gII6BMoAA</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/6156775075873092315?hl=pt-BR&amp;psb=1&amp;q=rtx+3060&amp;oq=rtx+3060&amp;gs_lcp=Cgtwcm9kdWN0cy1jYxAMUAxYHWA-aABwAHgAgAEAiAEAkgEAmAEAoAEBsAEA&amp;sclient=products-cc&amp;prds=eto:6583861436975444040_0,pid:5505575770092825149,rsk:PC_15471865893957977821&amp;sa=X&amp;ved=0ahUKEwjK95j9sMP-AhV-r5UCHcT0DKwQ8gII9RQoAA</t>
+  </si>
+  <si>
+    <t>https://www.pontofrio.com.br/placa-de-video-gigabyte-gaming-oc-12gb-geforce-rtx3060-gddr6-rgb-gv-n3060gaming-oc-12gd-1535614552/p/1535614552%3Futm_medium%3Dcpc%26utm_source%3Dgoogle_freelisting%26IdSku%3D1535614552%26idLojista%3D192053%26tipoLojista%3D3P&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiFsKD_sMP-AhUxl5UCHVGxDp44PBDVKQjhDSgA&amp;usg=AOvVaw1vFaRexRiK8oxQoTWk6wVJ</t>
+  </si>
+  <si>
+    <t>https://shopee.com.br/product/304224916/16586755093&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiFsKD_sMP-AhUxl5UCHVGxDp44PBDVKQjTDigA&amp;usg=AOvVaw20BwwU1bwU-W8SG70rdipg</t>
+  </si>
+  <si>
+    <t>https://www.enifler.com.br/pc-gamer-enifler-intel-core-i7-rtx-3060-16gb-ram-ssd-480gb-black-hawk&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwiFsKD_sMP-AhUxl5UCHVGxDp44PBDVKQjyDygA&amp;usg=AOvVaw01JhaYTbbJ35WJ93TKSSAE</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/14305462128264014099?q=rtx+3060&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;dpr=1&amp;prds=eto:11665494753858532241_0,pid:9462093140828316906,rsk:PC_10875814643528672174&amp;sa=X&amp;ved=0ahUKEwjf27eBscP-AhXQq5UCHfyIBos4eBDyAgjrDigA</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/12356433233958988052?q=rtx+3060&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;dpr=1&amp;prds=eto:16773169814766889904_0,pid:3966064649042890207&amp;sa=X&amp;ved=0ahUKEwiE5Y-IscP-AhXTnpUCHWZMA084rAIQ8gIItQ0oAA</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/6863560806293627420?q=rtx+3060&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;dpr=1&amp;prds=eto:4919617943665979035_0,pid:6596043544546096217&amp;sa=X&amp;ved=0ahUKEwiE5Y-IscP-AhXTnpUCHWZMA084rAIQ8gIIwg0oAA</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005004999142258.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjkvNGKscP-AhVLrpUCHeYSClE46AIQ1SkI0QwoAA&amp;usg=AOvVaw1jZGpyAw1bdjHvA1bzYmOJ</t>
+  </si>
+  <si>
+    <t>https://www.google.com.br/shopping/product/16910987619032744473?q=rtx+3060&amp;hl=pt-BR&amp;psb=1&amp;biw=1034&amp;bih=707&amp;dpr=1&amp;prds=eto:10838372646029017583_0,pid:6218787896921144287&amp;sa=X&amp;ved=0ahUKEwjkvNGKscP-AhVLrpUCHeYSClE46AIQ8gIIlA8oAA</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/deep_link.htm%3Faff_short_key%3DUneMJZVf%26dl_target_url%3Dhttps%253A%252F%252Fpt.aliexpress.com%252Fitem%252F1005003484105534.html%253F_randl_currency%253DBRL%2526_randl_shipto%253DBR%2526src%253Dgoogle&amp;rct=j&amp;q=&amp;esrc=s&amp;sa=U&amp;ved=0ahUKEwjdz4GNscP-AhX0kZUCHRbvDOk4pAMQ1SkIzA4oAA&amp;usg=AOvVaw0_OL0HX-0azvUiBtusDynp</t>
   </si>
   <si>
     <t>https://www.buscape.com.br/placa-de-video/placa-de-video-nvidia-geforce-rtx-3060-12-gb-gddr6-192-bits-asus-tuf-rtx3060-o12g-gaming?_lc=88&amp;searchterm=rtx%203060</t>
@@ -609,7 +645,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,10 +667,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -642,10 +678,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -653,10 +689,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -664,10 +700,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -675,10 +711,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -686,10 +722,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -697,10 +733,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -708,10 +744,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -719,10 +755,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -730,10 +766,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -741,10 +777,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -752,10 +788,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -763,10 +799,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -774,10 +810,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -785,10 +821,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -796,10 +832,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -807,10 +843,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -818,10 +854,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -829,10 +865,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -840,10 +876,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -851,10 +887,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -862,10 +898,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -873,10 +909,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -884,10 +920,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -895,10 +931,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -906,10 +942,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -917,10 +953,54 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -952,6 +1032,10 @@
     <hyperlink ref="C26" r:id="rId25"/>
     <hyperlink ref="C27" r:id="rId26"/>
     <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>